<commit_message>
edited informe 1 legendre es malo
</commit_message>
<xml_diff>
--- a/TP5/EJ1/Circuito con Bessel/Mediciones/Zin.xlsx
+++ b/TP5/EJ1/Circuito con Bessel/Mediciones/Zin.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41BC38B-A4B8-42B4-9A5A-EBC71822DE99}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75F15B9-B960-400B-94C1-0BDDFEE525F3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>relacion</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>Freq</t>
+  </si>
+  <si>
+    <t>ZIN ABS COPY</t>
+  </si>
+  <si>
+    <t>ZIN PHA COPY</t>
   </si>
 </sst>
 </file>
@@ -379,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G2" activeCellId="1" sqref="A2:A101 G2:G101"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -392,7 +398,7 @@
     <col min="5" max="5" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -420,8 +426,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>150</v>
       </c>
@@ -455,8 +467,14 @@
         <f>IMAGINARY(E2)</f>
         <v>-1065295.30749252</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L2">
+        <v>1077712.6598583618</v>
+      </c>
+      <c r="M2">
+        <v>-81.294002912317936</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>154.70918368633099</v>
       </c>
@@ -490,8 +508,14 @@
         <f t="shared" ref="I3:I66" si="5">IMAGINARY(E3)</f>
         <v>-1065295.30749252</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L3">
+        <v>1077712.6598583618</v>
+      </c>
+      <c r="M3">
+        <v>-81.294002912317936</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>159.566210112606</v>
       </c>
@@ -525,8 +549,14 @@
         <f t="shared" si="5"/>
         <v>-1065295.30749252</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L4">
+        <v>1077712.6598583618</v>
+      </c>
+      <c r="M4">
+        <v>-81.294002912317936</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>164.575720736286</v>
       </c>
@@ -560,8 +590,14 @@
         <f t="shared" si="5"/>
         <v>-1365026.3596105101</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <v>1415790.0821762078</v>
+      </c>
+      <c r="M5">
+        <v>-74.61061750252712</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>169.742502731336</v>
       </c>
@@ -595,8 +631,14 @@
         <f t="shared" si="5"/>
         <v>-1065295.30749252</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <v>1077712.6598583618</v>
+      </c>
+      <c r="M6">
+        <v>-81.294002912317936</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>175.07149356293201</v>
       </c>
@@ -630,8 +672,14 @@
         <f t="shared" si="5"/>
         <v>-932877.72519789101</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <v>956735.23917950178</v>
+      </c>
+      <c r="M7">
+        <v>-77.177846532606438</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>180.56778570578601</v>
       </c>
@@ -665,8 +713,14 @@
         <f t="shared" si="5"/>
         <v>-1044107.53472486</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <v>1073100.9823659612</v>
+      </c>
+      <c r="M8">
+        <v>-76.650961916420613</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>186.23663151060401</v>
       </c>
@@ -700,8 +754,14 @@
         <f t="shared" si="5"/>
         <v>-1365026.3596105101</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <v>1415790.0821762078</v>
+      </c>
+      <c r="M9">
+        <v>-74.61061750252712</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>192.08344822331699</v>
       </c>
@@ -735,8 +795,14 @@
         <f t="shared" si="5"/>
         <v>-1044107.53472486</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <v>1073100.9823659612</v>
+      </c>
+      <c r="M10">
+        <v>-76.650961916420613</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>198.1138231619</v>
       </c>
@@ -770,8 +836,14 @@
         <f t="shared" si="5"/>
         <v>-1044107.53472486</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <v>1073100.9823659612</v>
+      </c>
+      <c r="M11">
+        <v>-76.650961916420613</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>204.33351905570501</v>
       </c>
@@ -805,8 +877,14 @@
         <f t="shared" si="5"/>
         <v>-1044107.53472486</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <v>1073100.9823659612</v>
+      </c>
+      <c r="M12">
+        <v>-76.650961916420613</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>210.74847955242299</v>
       </c>
@@ -840,8 +918,14 @@
         <f t="shared" si="5"/>
         <v>-932877.72519789101</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>956735.23917950178</v>
+      </c>
+      <c r="M13">
+        <v>-77.177846532606438</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>217.36483489793901</v>
       </c>
@@ -875,8 +959,14 @@
         <f t="shared" si="5"/>
         <v>-932877.72519789101</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>956735.23917950178</v>
+      </c>
+      <c r="M14">
+        <v>-77.177846532606438</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>224.18890779449501</v>
       </c>
@@ -910,8 +1000,14 @@
         <f t="shared" si="5"/>
         <v>-932877.72519789101</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <v>956735.23917950178</v>
+      </c>
+      <c r="M15">
+        <v>-77.177846532606438</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>231.227219442777</v>
       </c>
@@ -945,8 +1041,14 @@
         <f t="shared" si="5"/>
         <v>-842551.29674343695</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>862995.81606083328</v>
+      </c>
+      <c r="M16">
+        <v>-77.503659183197144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>238.48649577368101</v>
       </c>
@@ -980,8 +1082,14 @@
         <f t="shared" si="5"/>
         <v>-842551.29674343695</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <v>862995.81606083328</v>
+      </c>
+      <c r="M17">
+        <v>-77.503659183197144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>245.973673875732</v>
       </c>
@@ -1015,8 +1123,14 @@
         <f t="shared" si="5"/>
         <v>-842551.29674343695</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L18">
+        <v>862995.81606083328</v>
+      </c>
+      <c r="M18">
+        <v>-77.503659183197144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>253.69590862428299</v>
       </c>
@@ -1050,8 +1164,14 @@
         <f t="shared" si="5"/>
         <v>-767825.60600962001</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <v>785918.48326332483</v>
+      </c>
+      <c r="M19">
+        <v>-77.682022528770716</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>261.66057951883198</v>
       </c>
@@ -1085,8 +1205,14 @@
         <f t="shared" si="5"/>
         <v>-767825.60600962001</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <v>785918.48326332483</v>
+      </c>
+      <c r="M20">
+        <v>-77.682022528770716</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>269.87529773500597</v>
       </c>
@@ -1120,8 +1246,14 @@
         <f t="shared" si="5"/>
         <v>-705024.19634377502</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <v>721453.23557613743</v>
+      </c>
+      <c r="M21">
+        <v>-77.749121439619486</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>278.34791339792201</v>
       </c>
@@ -1155,8 +1287,14 @@
         <f t="shared" si="5"/>
         <v>-694615.83684657305</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L22">
+        <v>720242.11884194613</v>
+      </c>
+      <c r="M22">
+        <v>-74.670169859270615</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>287.08652308390703</v>
       </c>
@@ -1190,8 +1328,14 @@
         <f t="shared" si="5"/>
         <v>-694615.83684657305</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L23">
+        <v>720242.11884194613</v>
+      </c>
+      <c r="M23">
+        <v>-74.670169859270615</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>296.09947755772203</v>
       </c>
@@ -1225,8 +1369,14 @@
         <f t="shared" si="5"/>
         <v>-598800.83135425404</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L24">
+        <v>619939.39972863032</v>
+      </c>
+      <c r="M24">
+        <v>-74.994771107407161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>305.39538975269602</v>
       </c>
@@ -1260,8 +1410,14 @@
         <f t="shared" si="5"/>
         <v>-598800.83135425404</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L25">
+        <v>619939.39972863032</v>
+      </c>
+      <c r="M25">
+        <v>-74.994771107407161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>314.98314300138998</v>
       </c>
@@ -1295,8 +1451,14 @@
         <f t="shared" si="5"/>
         <v>-598800.83135425404</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L26">
+        <v>619939.39972863032</v>
+      </c>
+      <c r="M26">
+        <v>-74.994771107407161</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>324.87189952466599</v>
       </c>
@@ -1330,8 +1492,14 @@
         <f t="shared" si="5"/>
         <v>-559879.96541138901</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L27">
+        <v>579555.42812486773</v>
+      </c>
+      <c r="M27">
+        <v>-75.027683400999308</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>335.07110918725903</v>
       </c>
@@ -1365,8 +1533,14 @@
         <f t="shared" si="5"/>
         <v>-559879.96541138901</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L28">
+        <v>579555.42812486773</v>
+      </c>
+      <c r="M28">
+        <v>-75.027683400999308</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>345.59051852822898</v>
       </c>
@@ -1400,8 +1574,14 @@
         <f t="shared" si="5"/>
         <v>-598800.83135425404</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L29">
+        <v>619939.39972863032</v>
+      </c>
+      <c r="M29">
+        <v>-74.994771107407161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>356.44018007492201</v>
       </c>
@@ -1435,8 +1615,14 @@
         <f t="shared" si="5"/>
         <v>-559879.96541138901</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L30">
+        <v>579555.42812486773</v>
+      </c>
+      <c r="M30">
+        <v>-75.027683400999308</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>367.63046194933298</v>
       </c>
@@ -1470,8 +1656,14 @@
         <f t="shared" si="5"/>
         <v>-552485.31709435105</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L31">
+        <v>579039.09177402919</v>
+      </c>
+      <c r="M31">
+        <v>-72.581104161041864</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>379.17205777606802</v>
       </c>
@@ -1505,8 +1697,14 @@
         <f t="shared" si="5"/>
         <v>-519431.861156289</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L32">
+        <v>544052.59299420076</v>
+      </c>
+      <c r="M32">
+        <v>-72.697086533384464</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>391.075996901346</v>
       </c>
@@ -1540,8 +1738,14 @@
         <f t="shared" si="5"/>
         <v>-519431.861156289</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L33">
+        <v>544052.59299420076</v>
+      </c>
+      <c r="M33">
+        <v>-72.697086533384464</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>403.35365493283598</v>
       </c>
@@ -1575,8 +1779,14 @@
         <f t="shared" si="5"/>
         <v>-489944.82120711601</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L34">
+        <v>513040.37608930975</v>
+      </c>
+      <c r="M34">
+        <v>-72.742857144960851</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>416.01676461037999</v>
       </c>
@@ -1610,8 +1820,14 @@
         <f t="shared" si="5"/>
         <v>-483498.29025253002</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L35">
+        <v>512596.25729606033</v>
+      </c>
+      <c r="M35">
+        <v>-70.601980794204991</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>429.07742701800402</v>
       </c>
@@ -1645,8 +1861,14 @@
         <f t="shared" si="5"/>
         <v>-483498.29025253002</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L36">
+        <v>512596.25729606033</v>
+      </c>
+      <c r="M36">
+        <v>-70.601980794204991</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>442.54812314791099</v>
       </c>
@@ -1680,8 +1902,14 @@
         <f t="shared" si="5"/>
         <v>-434951.30191765702</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L37">
+        <v>460728.40489714342</v>
+      </c>
+      <c r="M37">
+        <v>-70.743465510346041</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>456.44172582754197</v>
       </c>
@@ -1715,8 +1943,14 @@
         <f t="shared" si="5"/>
         <v>-434951.30191765702</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L38">
+        <v>460728.40489714342</v>
+      </c>
+      <c r="M38">
+        <v>-70.743465510346041</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>470.77151202106103</v>
       </c>
@@ -1750,8 +1984,14 @@
         <f t="shared" si="5"/>
         <v>-390626.53165651101</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L39">
+        <v>418564.04312584404</v>
+      </c>
+      <c r="M39">
+        <v>-68.947859117763457</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>485.55117551705399</v>
       </c>
@@ -1785,8 +2025,14 @@
         <f t="shared" si="5"/>
         <v>-373595.65130191803</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L40">
+        <v>400367.51010283077</v>
+      </c>
+      <c r="M40">
+        <v>-68.928388648015257</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>500.79484001454603</v>
       </c>
@@ -1820,8 +2066,14 @@
         <f t="shared" si="5"/>
         <v>-373595.65130191803</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L41">
+        <v>400367.51010283077</v>
+      </c>
+      <c r="M41">
+        <v>-68.928388648015257</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>516.51707261984802</v>
       </c>
@@ -1855,8 +2107,14 @@
         <f t="shared" si="5"/>
         <v>-354161.29652374203</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L42">
+        <v>383890.33045937447</v>
+      </c>
+      <c r="M42">
+        <v>-67.303034077675093</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>532.73289776713398</v>
       </c>
@@ -1890,8 +2148,14 @@
         <f t="shared" si="5"/>
         <v>-336334.77783248399</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L43">
+        <v>368786.37540771632</v>
+      </c>
+      <c r="M43">
+        <v>-65.783823918348475</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>549.45781157604699</v>
       </c>
@@ -1925,8 +2189,14 @@
         <f t="shared" si="5"/>
         <v>-323641.28759281</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L44">
+        <v>354897.92487419012</v>
+      </c>
+      <c r="M44">
+        <v>-65.773135061173321</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>566.70779666005399</v>
       </c>
@@ -1960,8 +2230,14 @@
         <f t="shared" si="5"/>
         <v>-323641.28759281</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L45">
+        <v>354897.92487419012</v>
+      </c>
+      <c r="M45">
+        <v>-65.773135061173321</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>584.49933739970902</v>
       </c>
@@ -1995,8 +2271,14 @@
         <f t="shared" si="5"/>
         <v>-308483.44947291003</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L46">
+        <v>342168.93892429082</v>
+      </c>
+      <c r="M46">
+        <v>-64.362965226722253</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>602.84943569540303</v>
       </c>
@@ -2030,8 +2312,14 @@
         <f t="shared" si="5"/>
         <v>-294472.245671955</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L47">
+        <v>330403.34180572932</v>
+      </c>
+      <c r="M47">
+        <v>-63.030846209732019</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>621.77562721467405</v>
       </c>
@@ -2065,8 +2353,14 @@
         <f t="shared" si="5"/>
         <v>-284672.90649345098</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L48">
+        <v>319458.20847064734</v>
+      </c>
+      <c r="M48">
+        <v>-63.013260610872294</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>641.29599814959204</v>
       </c>
@@ -2100,8 +2394,14 @@
         <f t="shared" si="5"/>
         <v>-281497.708843395</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L49">
+        <v>319505.55716564291</v>
+      </c>
+      <c r="M49">
+        <v>-61.768275547630509</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>661.42920250022803</v>
       </c>
@@ -2135,8 +2435,14 @@
         <f t="shared" si="5"/>
         <v>-269460.63662294601</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L50">
+        <v>309391.0032417138</v>
+      </c>
+      <c r="M50">
+        <v>-60.567920882301635</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>682.19447990074195</v>
       </c>
@@ -2170,8 +2476,14 @@
         <f t="shared" si="5"/>
         <v>-261263.59262257701</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L51">
+        <v>299985.36966070416</v>
+      </c>
+      <c r="M51">
+        <v>-60.565856054266952</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>703.61167400509999</v>
       </c>
@@ -2205,8 +2517,14 @@
         <f t="shared" si="5"/>
         <v>-250742.500214528</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L52">
+        <v>291232.56652238377</v>
+      </c>
+      <c r="M52">
+        <v>-59.425668503941552</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>725.70125145001305</v>
       </c>
@@ -2240,8 +2558,14 @@
         <f t="shared" si="5"/>
         <v>-247851.99047914601</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L53">
+        <v>291220.65009764605</v>
+      </c>
+      <c r="M53">
+        <v>-58.329301011642542</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>748.484321413202</v>
       </c>
@@ -2275,8 +2599,14 @@
         <f t="shared" si="5"/>
         <v>-238129.44700881801</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L54">
+        <v>283039.68182531523</v>
+      </c>
+      <c r="M54">
+        <v>-57.280708940100794</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>771.98265578569396</v>
       </c>
@@ -2310,8 +2640,14 @@
         <f t="shared" si="5"/>
         <v>-229040.697470099</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L55">
+        <v>275389.62584224035</v>
+      </c>
+      <c r="M55">
+        <v>-56.273447050112274</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>796.21870997740496</v>
       </c>
@@ -2345,8 +2681,14 @@
         <f t="shared" si="5"/>
         <v>-226249.46010537801</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L56">
+        <v>275286.56896783621</v>
+      </c>
+      <c r="M56">
+        <v>-55.272314300276307</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>821.21564437591906</v>
       </c>
@@ -2380,8 +2722,14 @@
         <f t="shared" si="5"/>
         <v>-217853.70422231301</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L57">
+        <v>268131.15457317198</v>
+      </c>
+      <c r="M57">
+        <v>-54.339864393009108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>846.99734647895104</v>
       </c>
@@ -2415,8 +2763,14 @@
         <f t="shared" si="5"/>
         <v>-209979.91373964201</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L58">
+        <v>261420.02709892963</v>
+      </c>
+      <c r="M58">
+        <v>-53.439479137301106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>873.58845372164797</v>
       </c>
@@ -2450,8 +2804,14 @@
         <f t="shared" si="5"/>
         <v>-202582.27373258499</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L59">
+        <v>255115.59501414662</v>
+      </c>
+      <c r="M59">
+        <v>-52.568475812317622</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>901.01437702053602</v>
       </c>
@@ -2485,8 +2845,14 @@
         <f t="shared" si="5"/>
         <v>-195619.876205437</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L60">
+        <v>249184.26046019953</v>
+      </c>
+      <c r="M60">
+        <v>-51.724476057767028</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>929.30132505663505</v>
       </c>
@@ -2520,8 +2886,14 @@
         <f t="shared" si="5"/>
         <v>-186750.169374171</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L61">
+        <v>243503.46323570731</v>
+      </c>
+      <c r="M61">
+        <v>-50.07902167440885</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>958.47632932091994</v>
       </c>
@@ -2555,8 +2927,14 @@
         <f t="shared" si="5"/>
         <v>-180651.484631019</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L62">
+        <v>238248.67560113879</v>
+      </c>
+      <c r="M62">
+        <v>-49.309952100789424</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>988.56726994607004</v>
       </c>
@@ -2590,8 +2968,14 @@
         <f t="shared" si="5"/>
         <v>-172735.335304543</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L63">
+        <v>233186.00112305733</v>
+      </c>
+      <c r="M63">
+        <v>-47.796369255245118</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>1019.60290234921</v>
       </c>
@@ -2625,8 +3009,14 @@
         <f t="shared" si="5"/>
         <v>-167365.26784970099</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L64">
+        <v>228510.85725144425</v>
+      </c>
+      <c r="M64">
+        <v>-47.089415776983003</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>1051.6128847110599</v>
       </c>
@@ -2660,8 +3050,14 @@
         <f t="shared" si="5"/>
         <v>-163173.70264947499</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L65">
+        <v>228243.93985114034</v>
+      </c>
+      <c r="M65">
+        <v>-45.63576193116603</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>1084.6278063178399</v>
       </c>
@@ -2695,8 +3091,14 @@
         <f t="shared" si="5"/>
         <v>-158263.310448173</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L66">
+        <v>223861.96152912441</v>
+      </c>
+      <c r="M66">
+        <v>-44.988780205809853</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>1118.67921679286</v>
       </c>
@@ -2707,31 +3109,37 @@
         <v>-43</v>
       </c>
       <c r="D67" t="str">
-        <f t="shared" ref="D67:D130" si="6">COMPLEX((10^(B67/20))*COS(RADIANS(C67)),(10^(B67/20))*SIN(RADIANS(C67)),"j")</f>
+        <f t="shared" ref="D67:D101" si="6">COMPLEX((10^(B67/20))*COS(RADIANS(C67)),(10^(B67/20))*SIN(RADIANS(C67)),"j")</f>
         <v>0.505973141476349-0.471827587607161j</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E130" si="7">IMDIV(150000,(IMSUB(1,D67)))</f>
+        <f t="shared" ref="E67:E101" si="7">IMDIV(150000,(IMSUB(1,D67)))</f>
         <v>158788.51438749-151653.296557737j</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F130" si="8">IMABS(E67)</f>
+        <f t="shared" ref="F67:F101" si="8">IMABS(E67)</f>
         <v>219573.4835043044</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G130" si="9">DEGREES(IMARGUMENT(E67))</f>
+        <f t="shared" ref="G67:G101" si="9">DEGREES(IMARGUMENT(E67))</f>
         <v>-43.683341329922484</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:H130" si="10">IMREAL(E67)</f>
+        <f t="shared" ref="H67:H101" si="10">IMREAL(E67)</f>
         <v>158788.51438748999</v>
       </c>
       <c r="I67">
-        <f t="shared" ref="I67:I130" si="11">IMAGINARY(E67)</f>
+        <f t="shared" ref="I67:I101" si="11">IMAGINARY(E67)</f>
         <v>-151653.29655773699</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L67">
+        <v>219573.4835043044</v>
+      </c>
+      <c r="M67">
+        <v>-43.683341329922484</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>1153.79965624592</v>
       </c>
@@ -2765,8 +3173,14 @@
         <f t="shared" si="11"/>
         <v>-145425.04529109999</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L68">
+        <v>215516.03914336726</v>
+      </c>
+      <c r="M68">
+        <v>-42.436755739179411</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>1190.0226863691701</v>
       </c>
@@ -2800,8 +3214,14 @@
         <f t="shared" si="11"/>
         <v>-143544.2339807</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L69">
+        <v>215353.96337797111</v>
+      </c>
+      <c r="M69">
+        <v>-41.801365050088556</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>1227.38292250926</v>
       </c>
@@ -2835,8 +3255,14 @@
         <f t="shared" si="11"/>
         <v>-137747.27783520299</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L70">
+        <v>211516.68968072199</v>
+      </c>
+      <c r="M70">
+        <v>-40.634854108757516</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>1265.91606674635</v>
       </c>
@@ -2870,8 +3296,14 @@
         <f t="shared" si="11"/>
         <v>-134124.789918967</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L71">
+        <v>211133.74729009726</v>
+      </c>
+      <c r="M71">
+        <v>-39.439258766961373</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>1305.6589420115899</v>
       </c>
@@ -2905,8 +3337,14 @@
         <f t="shared" si="11"/>
         <v>-128811.83428691499</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L72">
+        <v>207518.33146074356</v>
+      </c>
+      <c r="M72">
+        <v>-38.369103499782838</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>1346.64952727581</v>
       </c>
@@ -2940,8 +3378,14 @@
         <f t="shared" si="11"/>
         <v>-122245.801590167</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L73">
+        <v>201199.02729625415</v>
+      </c>
+      <c r="M73">
+        <v>-37.415191029943777</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>1388.9269938428299</v>
       </c>
@@ -2975,8 +3419,14 @@
         <f t="shared" si="11"/>
         <v>-120490.650470309</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L74">
+        <v>203684.77708271</v>
+      </c>
+      <c r="M74">
+        <v>-36.267399402807214</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>1432.5317427822299</v>
       </c>
@@ -3010,8 +3460,14 @@
         <f t="shared" si="11"/>
         <v>-115905.04638669601</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L75">
+        <v>200474.93115692554</v>
+      </c>
+      <c r="M75">
+        <v>-35.320691275411093</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>1477.5054435372999</v>
       </c>
@@ -3045,8 +3501,14 @@
         <f t="shared" si="11"/>
         <v>-111570.975361416</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L76">
+        <v>197438.25906580538</v>
+      </c>
+      <c r="M76">
+        <v>-34.408748670183009</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>1523.8910737451099</v>
       </c>
@@ -3080,8 +3542,14 @@
         <f t="shared" si="11"/>
         <v>-107469.763857201</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L77">
+        <v>194563.68967096531</v>
+      </c>
+      <c r="M77">
+        <v>-33.529269283091814</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>1571.73296030662</v>
       </c>
@@ -3115,8 +3583,14 @@
         <f t="shared" si="11"/>
         <v>-104608.28295363201</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L78">
+        <v>194178.74195803629</v>
+      </c>
+      <c r="M78">
+        <v>-32.596655095663692</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>1621.0768217462501</v>
       </c>
@@ -3150,8 +3624,14 @@
         <f t="shared" si="11"/>
         <v>-100850.09535275299</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L79">
+        <v>191483.99902355304</v>
+      </c>
+      <c r="M79">
+        <v>-31.781163600321378</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>1671.9698119013001</v>
       </c>
@@ -3185,8 +3665,14 @@
         <f t="shared" si="11"/>
         <v>-98150.583430408806</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L80">
+        <v>191091.23843389601</v>
+      </c>
+      <c r="M80">
+        <v>-30.906062679763846</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>1724.46056498292</v>
       </c>
@@ -3220,8 +3706,14 @@
         <f t="shared" si="11"/>
         <v>-95490.256146368905</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L81">
+        <v>190666.26599825255</v>
+      </c>
+      <c r="M81">
+        <v>-30.054535301770983</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>1778.5992420518501</v>
       </c>
@@ -3255,8 +3747,14 @@
         <f t="shared" si="11"/>
         <v>-90910.7640907202</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L82">
+        <v>187969.42436043106</v>
+      </c>
+      <c r="M82">
+        <v>-28.923836219577574</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>1834.43757895313</v>
       </c>
@@ -3290,8 +3788,14 @@
         <f t="shared" si="11"/>
         <v>-88434.328622942601</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L83">
+        <v>187538.31041102414</v>
+      </c>
+      <c r="M83">
+        <v>-28.13517866873207</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>1892.0289357557799</v>
       </c>
@@ -3325,8 +3829,14 @@
         <f t="shared" si="11"/>
         <v>-85441.9301961397</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L84">
+        <v>185228.08924077768</v>
+      </c>
+      <c r="M84">
+        <v>-27.469705580097511</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>1951.4283477446299</v>
       </c>
@@ -3360,8 +3870,14 @@
         <f t="shared" si="11"/>
         <v>-81977.442785516803</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L85">
+        <v>184594.3927169932</v>
+      </c>
+      <c r="M85">
+        <v>-26.365450253628691</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>2012.69257801292</v>
       </c>
@@ -3395,8 +3911,14 @@
         <f t="shared" si="11"/>
         <v>-79282.007643244098</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L86">
+        <v>182454.30997578308</v>
+      </c>
+      <c r="M86">
+        <v>-25.755438354686625</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>2075.8801717061101</v>
       </c>
@@ -3430,8 +3952,14 @@
         <f t="shared" si="11"/>
         <v>-77130.372726736605</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L87">
+        <v>182045.32152795314</v>
+      </c>
+      <c r="M87">
+        <v>-25.067630514915233</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>2141.0515119686202</v>
       </c>
@@ -3465,8 +3993,14 @@
         <f t="shared" si="11"/>
         <v>-75024.773617104001</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L88">
+        <v>181622.29286118617</v>
+      </c>
+      <c r="M88">
+        <v>-24.398545060277737</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2208.268877647</v>
       </c>
@@ -3500,8 +4034,14 @@
         <f t="shared" si="11"/>
         <v>-72966.052201076804</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L89">
+        <v>181187.08251537051</v>
+      </c>
+      <c r="M89">
+        <v>-23.747773199961049</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>2277.5965028046498</v>
       </c>
@@ -3535,8 +4075,14 @@
         <f t="shared" si="11"/>
         <v>-71212.635601615199</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L90">
+        <v>182242.5782938723</v>
+      </c>
+      <c r="M90">
+        <v>-23.001635092538308</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>2349.1006381050101</v>
       </c>
@@ -3570,8 +4116,14 @@
         <f t="shared" si="11"/>
         <v>-68027.670384285404</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L91">
+        <v>180056.8327893026</v>
+      </c>
+      <c r="M91">
+        <v>-22.198231746836932</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>2422.8496141217702</v>
       </c>
@@ -3605,8 +4157,14 @@
         <f t="shared" si="11"/>
         <v>-66136.256266708602</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L92">
+        <v>179591.84452269485</v>
+      </c>
+      <c r="M92">
+        <v>-21.608265815022435</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>2498.9139066368102</v>
       </c>
@@ -3640,8 +4198,14 @@
         <f t="shared" si="11"/>
         <v>-64292.757337319097</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L93">
+        <v>179121.54771915384</v>
+      </c>
+      <c r="M93">
+        <v>-21.03472445902592</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>2577.3662039880001</v>
       </c>
@@ -3675,8 +4239,14 @@
         <f t="shared" si="11"/>
         <v>-62673.715741171</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L94">
+        <v>181268.47422416843</v>
+      </c>
+      <c r="M94">
+        <v>-20.227632693364047</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>2658.2814765314802</v>
       </c>
@@ -3710,8 +4280,14 @@
         <f t="shared" si="11"/>
         <v>-60869.887231801797</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L95">
+        <v>180709.42584265923</v>
+      </c>
+      <c r="M95">
+        <v>-19.684373438273923</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>2741.7370482845399</v>
       </c>
@@ -3745,8 +4321,14 @@
         <f t="shared" si="11"/>
         <v>-58259.772812683899</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L96">
+        <v>179872.16037297508</v>
+      </c>
+      <c r="M96">
+        <v>-18.898669081794246</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>2827.8126708178102</v>
       </c>
@@ -3780,8 +4362,14 @@
         <f t="shared" si="11"/>
         <v>-56582.1888022864</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L97">
+        <v>179316.15967160516</v>
+      </c>
+      <c r="M97">
+        <v>-18.393674702711838</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>2916.5905994672498</v>
       </c>
@@ -3815,8 +4403,14 @@
         <f t="shared" si="11"/>
         <v>-54953.497460881998</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L98">
+        <v>178762.83206885803</v>
+      </c>
+      <c r="M98">
+        <v>-17.903219325221706</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>3008.1556719386999</v>
       </c>
@@ -3850,8 +4444,14 @@
         <f t="shared" si="11"/>
         <v>-53372.691126995502</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L99">
+        <v>178212.88794370918</v>
+      </c>
+      <c r="M99">
+        <v>-17.426877322181099</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>3102.5953893802898</v>
       </c>
@@ -3885,8 +4485,14 @@
         <f t="shared" si="11"/>
         <v>-51838.718029858399</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L100">
+        <v>177666.96514221444</v>
+      </c>
+      <c r="M100">
+        <v>-16.964232130886909</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>3199.99999999999</v>
       </c>
@@ -3919,6 +4525,12 @@
       <c r="I101">
         <f t="shared" si="11"/>
         <v>-50240.912972202401</v>
+      </c>
+      <c r="L101">
+        <v>178165.28777603325</v>
+      </c>
+      <c r="M101">
+        <v>-16.37903807463735</v>
       </c>
     </row>
   </sheetData>

</xml_diff>